<commit_message>
conta quantas vezes cada palavra aparece
</commit_message>
<xml_diff>
--- a/Projeto 2/Rick_and_Morty.xlsx
+++ b/Projeto 2/Rick_and_Morty.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User-pc\Documents\GitHub\Ciencia-dos-Dados\Projeto 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucca\Desktop\Ciencia-dos-Dados-master\Projeto 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="2532" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1386,7 +1386,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1708,17 +1708,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
-      <selection activeCell="O291" sqref="O291"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="3.44140625" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="6.77734375" hidden="1" customWidth="1"/>
+    <col min="10" max="12" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="24.88671875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1731,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1734,15 +1739,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="O3" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="165" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="144" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1750,7 +1755,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1758,7 +1763,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1766,7 +1771,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1774,7 +1779,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1782,7 +1787,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1790,7 +1795,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1798,7 +1803,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1806,7 +1811,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1814,7 +1819,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1822,7 +1827,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1830,7 +1835,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1838,15 +1843,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="O16" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -1854,15 +1859,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
       <c r="O18" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -1870,15 +1875,15 @@
         <v>403</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>2</v>
       </c>
       <c r="O20" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1886,7 +1891,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1894,7 +1899,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1902,7 +1907,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1910,7 +1915,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1918,7 +1923,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1926,7 +1931,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1934,7 +1939,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -1942,15 +1947,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
       <c r="O29" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -1958,7 +1963,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -1966,7 +1971,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1974,7 +1979,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>28</v>
       </c>
@@ -1982,7 +1987,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1990,7 +1995,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -1998,7 +2003,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -2006,7 +2011,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -2014,7 +2019,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -2022,7 +2027,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>32</v>
       </c>
@@ -2030,7 +2035,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>33</v>
       </c>
@@ -2038,7 +2043,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>34</v>
       </c>
@@ -2046,7 +2051,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -2054,7 +2059,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -2062,7 +2067,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -2070,7 +2075,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>38</v>
       </c>
@@ -2078,7 +2083,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -2086,7 +2091,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>40</v>
       </c>
@@ -2094,7 +2099,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -2102,7 +2107,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -2110,7 +2115,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -2118,7 +2123,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>44</v>
       </c>
@@ -2126,7 +2131,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>45</v>
       </c>
@@ -2134,7 +2139,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>46</v>
       </c>
@@ -2142,15 +2147,15 @@
         <v>403</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>2</v>
       </c>
       <c r="O54" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>47</v>
       </c>
@@ -2158,7 +2163,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>48</v>
       </c>
@@ -2166,7 +2171,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>49</v>
       </c>
@@ -2174,7 +2179,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>26</v>
       </c>
@@ -2182,7 +2187,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>50</v>
       </c>
@@ -2190,7 +2195,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>51</v>
       </c>
@@ -2198,7 +2203,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>52</v>
       </c>
@@ -2206,7 +2211,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>53</v>
       </c>
@@ -2214,7 +2219,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>54</v>
       </c>
@@ -2222,7 +2227,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -2230,7 +2235,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>56</v>
       </c>
@@ -2238,7 +2243,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>57</v>
       </c>
@@ -2246,7 +2251,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>58</v>
       </c>
@@ -2254,7 +2259,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>59</v>
       </c>
@@ -2262,7 +2267,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>60</v>
       </c>
@@ -2270,7 +2275,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>61</v>
       </c>
@@ -2278,7 +2283,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>26</v>
       </c>
@@ -2286,7 +2291,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>62</v>
       </c>
@@ -2294,7 +2299,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>9</v>
       </c>
@@ -2302,15 +2307,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>14</v>
       </c>
       <c r="O74" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>63</v>
       </c>
@@ -2318,7 +2323,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>9</v>
       </c>
@@ -2326,7 +2331,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>64</v>
       </c>
@@ -2334,7 +2339,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>9</v>
       </c>
@@ -2342,7 +2347,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>65</v>
       </c>
@@ -2350,7 +2355,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>66</v>
       </c>
@@ -2358,7 +2363,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>9</v>
       </c>
@@ -2366,7 +2371,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>67</v>
       </c>
@@ -2374,7 +2379,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>68</v>
       </c>
@@ -2382,7 +2387,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>69</v>
       </c>
@@ -2390,7 +2395,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>70</v>
       </c>
@@ -2398,7 +2403,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>71</v>
       </c>
@@ -2406,7 +2411,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>72</v>
       </c>
@@ -2414,7 +2419,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>73</v>
       </c>
@@ -2422,7 +2427,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>74</v>
       </c>
@@ -2430,7 +2435,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>75</v>
       </c>
@@ -2438,7 +2443,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>76</v>
       </c>
@@ -2446,7 +2451,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>2</v>
       </c>
@@ -2454,7 +2459,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>77</v>
       </c>
@@ -2462,7 +2467,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>78</v>
       </c>
@@ -2470,7 +2475,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>79</v>
       </c>
@@ -2478,7 +2483,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>80</v>
       </c>
@@ -2486,7 +2491,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>81</v>
       </c>
@@ -2494,7 +2499,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>82</v>
       </c>
@@ -2502,7 +2507,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>83</v>
       </c>
@@ -2510,7 +2515,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>9</v>
       </c>
@@ -2518,7 +2523,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>84</v>
       </c>
@@ -2526,7 +2531,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>85</v>
       </c>
@@ -2534,7 +2539,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>86</v>
       </c>
@@ -2542,7 +2547,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>87</v>
       </c>
@@ -2550,15 +2555,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>88</v>
       </c>
       <c r="O105" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>89</v>
       </c>
@@ -2566,7 +2571,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>90</v>
       </c>
@@ -2574,15 +2579,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>13</v>
       </c>
       <c r="O108" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>26</v>
       </c>
@@ -2590,7 +2595,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>91</v>
       </c>
@@ -2598,7 +2603,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>92</v>
       </c>
@@ -2606,7 +2611,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>59</v>
       </c>
@@ -2614,7 +2619,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>26</v>
       </c>
@@ -2622,7 +2627,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>93</v>
       </c>
@@ -2630,7 +2635,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>94</v>
       </c>
@@ -2638,7 +2643,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>95</v>
       </c>
@@ -2646,7 +2651,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>96</v>
       </c>
@@ -2654,7 +2659,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>9</v>
       </c>
@@ -2662,7 +2667,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>97</v>
       </c>
@@ -2670,7 +2675,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>95</v>
       </c>
@@ -2678,7 +2683,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>98</v>
       </c>
@@ -2686,7 +2691,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>99</v>
       </c>
@@ -2694,7 +2699,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>100</v>
       </c>
@@ -2702,7 +2707,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>101</v>
       </c>
@@ -2710,7 +2715,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>102</v>
       </c>
@@ -2718,7 +2723,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>103</v>
       </c>
@@ -2726,7 +2731,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>104</v>
       </c>
@@ -2734,7 +2739,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>105</v>
       </c>
@@ -2742,7 +2747,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>106</v>
       </c>
@@ -2750,7 +2755,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>107</v>
       </c>
@@ -2758,7 +2763,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>108</v>
       </c>
@@ -2766,7 +2771,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>109</v>
       </c>
@@ -2774,7 +2779,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>110</v>
       </c>
@@ -2782,7 +2787,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>111</v>
       </c>
@@ -2790,7 +2795,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>112</v>
       </c>
@@ -2798,7 +2803,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>113</v>
       </c>
@@ -2806,7 +2811,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>114</v>
       </c>
@@ -2814,7 +2819,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>115</v>
       </c>
@@ -2822,7 +2827,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>116</v>
       </c>
@@ -2830,7 +2835,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>24</v>
       </c>
@@ -2838,7 +2843,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>117</v>
       </c>
@@ -2846,7 +2851,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>118</v>
       </c>
@@ -2854,7 +2859,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>14</v>
       </c>
@@ -2862,7 +2867,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>9</v>
       </c>
@@ -2870,7 +2875,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>119</v>
       </c>
@@ -2878,7 +2883,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>120</v>
       </c>
@@ -2886,7 +2891,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>9</v>
       </c>
@@ -2894,7 +2899,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>121</v>
       </c>
@@ -2902,7 +2907,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>122</v>
       </c>
@@ -2910,7 +2915,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>26</v>
       </c>
@@ -2918,7 +2923,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>123</v>
       </c>
@@ -2926,7 +2931,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>124</v>
       </c>
@@ -2934,7 +2939,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>125</v>
       </c>
@@ -2942,7 +2947,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>126</v>
       </c>
@@ -2950,7 +2955,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>127</v>
       </c>
@@ -2958,7 +2963,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>128</v>
       </c>
@@ -2966,7 +2971,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>129</v>
       </c>
@@ -2974,7 +2979,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>130</v>
       </c>
@@ -2982,7 +2987,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>131</v>
       </c>
@@ -2990,7 +2995,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>132</v>
       </c>
@@ -2998,7 +3003,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>133</v>
       </c>
@@ -3006,7 +3011,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>134</v>
       </c>
@@ -3014,7 +3019,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>135</v>
       </c>
@@ -3022,7 +3027,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>136</v>
       </c>
@@ -3030,7 +3035,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>2</v>
       </c>
@@ -3038,7 +3043,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>137</v>
       </c>
@@ -3046,23 +3051,23 @@
         <v>403</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>14</v>
       </c>
       <c r="O167" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>2</v>
       </c>
       <c r="O168" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>138</v>
       </c>
@@ -3070,7 +3075,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>139</v>
       </c>
@@ -3078,15 +3083,15 @@
         <v>403</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>14</v>
       </c>
       <c r="O171" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>95</v>
       </c>
@@ -3094,7 +3099,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>140</v>
       </c>
@@ -3102,15 +3107,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>141</v>
       </c>
       <c r="O174" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>142</v>
       </c>
@@ -3118,7 +3123,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>143</v>
       </c>
@@ -3126,7 +3131,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>144</v>
       </c>
@@ -3134,7 +3139,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>145</v>
       </c>
@@ -3142,7 +3147,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>146</v>
       </c>
@@ -3150,7 +3155,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>147</v>
       </c>
@@ -3158,7 +3163,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>148</v>
       </c>
@@ -3166,7 +3171,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>149</v>
       </c>
@@ -3174,7 +3179,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>150</v>
       </c>
@@ -3182,7 +3187,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>151</v>
       </c>
@@ -3190,7 +3195,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>152</v>
       </c>
@@ -3198,7 +3203,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>153</v>
       </c>
@@ -3206,7 +3211,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>154</v>
       </c>
@@ -3214,7 +3219,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>155</v>
       </c>
@@ -3222,7 +3227,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>156</v>
       </c>
@@ -3230,7 +3235,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>157</v>
       </c>
@@ -3238,7 +3243,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>26</v>
       </c>
@@ -3246,7 +3251,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>158</v>
       </c>
@@ -3254,7 +3259,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>159</v>
       </c>
@@ -3262,7 +3267,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>160</v>
       </c>
@@ -3270,7 +3275,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>161</v>
       </c>
@@ -3278,7 +3283,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>162</v>
       </c>
@@ -3286,15 +3291,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>163</v>
       </c>
       <c r="O197" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>164</v>
       </c>
@@ -3302,7 +3307,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>165</v>
       </c>
@@ -3310,7 +3315,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>166</v>
       </c>
@@ -3318,7 +3323,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>167</v>
       </c>
@@ -3326,7 +3331,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>168</v>
       </c>
@@ -3334,7 +3339,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>169</v>
       </c>
@@ -3342,7 +3347,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>95</v>
       </c>
@@ -3350,7 +3355,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>170</v>
       </c>
@@ -3358,7 +3363,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>171</v>
       </c>
@@ -3366,7 +3371,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>26</v>
       </c>
@@ -3374,7 +3379,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>172</v>
       </c>
@@ -3382,7 +3387,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>173</v>
       </c>
@@ -3390,7 +3395,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>20</v>
       </c>
@@ -3398,7 +3403,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>9</v>
       </c>
@@ -3406,7 +3411,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>174</v>
       </c>
@@ -3414,7 +3419,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>175</v>
       </c>
@@ -3422,7 +3427,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>176</v>
       </c>
@@ -3430,7 +3435,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>177</v>
       </c>
@@ -3438,7 +3443,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>178</v>
       </c>
@@ -3446,7 +3451,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>179</v>
       </c>
@@ -3454,7 +3459,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>9</v>
       </c>
@@ -3462,7 +3467,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>180</v>
       </c>
@@ -3470,7 +3475,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>9</v>
       </c>
@@ -3478,7 +3483,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>181</v>
       </c>
@@ -3486,15 +3491,15 @@
         <v>403</v>
       </c>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>2</v>
       </c>
       <c r="O222" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="223" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>142</v>
       </c>
@@ -3502,7 +3507,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>59</v>
       </c>
@@ -3510,7 +3515,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>9</v>
       </c>
@@ -3518,7 +3523,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>182</v>
       </c>
@@ -3526,7 +3531,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>183</v>
       </c>
@@ -3534,7 +3539,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>184</v>
       </c>
@@ -3542,7 +3547,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>185</v>
       </c>
@@ -3550,7 +3555,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>186</v>
       </c>
@@ -3558,7 +3563,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>9</v>
       </c>
@@ -3566,7 +3571,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>9</v>
       </c>
@@ -3574,7 +3579,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>187</v>
       </c>
@@ -3582,7 +3587,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>188</v>
       </c>
@@ -3590,7 +3595,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>24</v>
       </c>
@@ -3598,7 +3603,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>189</v>
       </c>
@@ -3606,7 +3611,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>9</v>
       </c>
@@ -3614,7 +3619,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>2</v>
       </c>
@@ -3622,7 +3627,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>190</v>
       </c>
@@ -3630,7 +3635,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>191</v>
       </c>
@@ -3638,7 +3643,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>2</v>
       </c>
@@ -3646,7 +3651,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>192</v>
       </c>
@@ -3654,7 +3659,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>193</v>
       </c>
@@ -3662,7 +3667,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>26</v>
       </c>
@@ -3670,7 +3675,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>194</v>
       </c>
@@ -3678,7 +3683,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>195</v>
       </c>
@@ -3686,7 +3691,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>9</v>
       </c>
@@ -3694,7 +3699,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>196</v>
       </c>
@@ -3702,7 +3707,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>197</v>
       </c>
@@ -3710,7 +3715,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>198</v>
       </c>
@@ -3718,7 +3723,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>199</v>
       </c>
@@ -3726,7 +3731,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>200</v>
       </c>
@@ -3734,7 +3739,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>81</v>
       </c>
@@ -3742,7 +3747,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>201</v>
       </c>
@@ -3750,7 +3755,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>202</v>
       </c>
@@ -3758,7 +3763,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>203</v>
       </c>
@@ -3766,15 +3771,15 @@
         <v>403</v>
       </c>
     </row>
-    <row r="257" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>204</v>
       </c>
       <c r="O257" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="258" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="258" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>205</v>
       </c>
@@ -3782,23 +3787,23 @@
         <v>403</v>
       </c>
     </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>206</v>
       </c>
       <c r="O259" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="260" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="260" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>2</v>
       </c>
       <c r="O260" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="261" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="261" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>207</v>
       </c>
@@ -3806,7 +3811,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="262" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>208</v>
       </c>
@@ -3814,7 +3819,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="263" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>209</v>
       </c>
@@ -3822,7 +3827,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="264" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>210</v>
       </c>
@@ -3830,7 +3835,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="265" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>211</v>
       </c>
@@ -3838,15 +3843,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="266" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>2</v>
       </c>
       <c r="O266" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="267" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="267" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>212</v>
       </c>
@@ -3854,15 +3859,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="268" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>213</v>
       </c>
       <c r="O268" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="269" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="269" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>214</v>
       </c>
@@ -3870,7 +3875,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="270" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>215</v>
       </c>
@@ -3878,7 +3883,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="271" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>216</v>
       </c>
@@ -3886,7 +3891,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="272" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>217</v>
       </c>
@@ -3894,7 +3899,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>218</v>
       </c>
@@ -3902,7 +3907,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>219</v>
       </c>
@@ -3910,7 +3915,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>220</v>
       </c>
@@ -3918,7 +3923,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>26</v>
       </c>
@@ -3926,7 +3931,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>221</v>
       </c>
@@ -3934,7 +3939,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>222</v>
       </c>
@@ -3942,7 +3947,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>223</v>
       </c>
@@ -3950,7 +3955,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>224</v>
       </c>
@@ -3958,7 +3963,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>225</v>
       </c>
@@ -3966,7 +3971,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>226</v>
       </c>
@@ -3974,15 +3979,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="283" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>59</v>
       </c>
       <c r="O283" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="284" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>227</v>
       </c>
@@ -3990,7 +3995,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>228</v>
       </c>
@@ -3998,7 +4003,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>229</v>
       </c>
@@ -4006,7 +4011,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>230</v>
       </c>
@@ -4014,7 +4019,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>231</v>
       </c>
@@ -4022,7 +4027,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="289" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>232</v>
       </c>
@@ -4030,7 +4035,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="290" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>26</v>
       </c>
@@ -4038,7 +4043,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="291" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>233</v>
       </c>
@@ -4046,7 +4051,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="292" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>234</v>
       </c>
@@ -4054,15 +4059,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="293" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>2</v>
       </c>
       <c r="O293" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="294" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>235</v>
       </c>
@@ -4070,7 +4075,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="295" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>236</v>
       </c>
@@ -4078,7 +4083,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="296" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>9</v>
       </c>
@@ -4086,15 +4091,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="297" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>237</v>
       </c>
       <c r="O297" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="298" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="298" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>238</v>
       </c>
@@ -4102,23 +4107,23 @@
         <v>402</v>
       </c>
     </row>
-    <row r="299" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>95</v>
       </c>
       <c r="O299" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="300" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="300" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>9</v>
       </c>
       <c r="O300" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="301" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="301" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>239</v>
       </c>
@@ -4138,16 +4143,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O201"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="O202" activeCellId="1" sqref="O201 O202"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="1.33203125" customWidth="1"/>
+    <col min="7" max="13" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>240</v>
       </c>
@@ -4155,7 +4163,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -4163,7 +4171,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>241</v>
       </c>
@@ -4171,7 +4179,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>242</v>
       </c>
@@ -4179,7 +4187,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>243</v>
       </c>
@@ -4187,7 +4195,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>244</v>
       </c>
@@ -4195,7 +4203,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>245</v>
       </c>
@@ -4203,7 +4211,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -4211,7 +4219,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>246</v>
       </c>
@@ -4219,7 +4227,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>247</v>
       </c>
@@ -4227,7 +4235,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>248</v>
       </c>
@@ -4235,7 +4243,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>95</v>
       </c>
@@ -4243,15 +4251,15 @@
         <v>404</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>249</v>
       </c>
       <c r="O13" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>250</v>
       </c>
@@ -4259,7 +4267,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>251</v>
       </c>
@@ -4267,7 +4275,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>252</v>
       </c>
@@ -4275,7 +4283,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>253</v>
       </c>
@@ -4283,7 +4291,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>254</v>
       </c>
@@ -4291,7 +4299,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>255</v>
       </c>
@@ -4299,7 +4307,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>256</v>
       </c>
@@ -4307,7 +4315,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>257</v>
       </c>
@@ -4315,15 +4323,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>141</v>
       </c>
       <c r="O22" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>258</v>
       </c>
@@ -4331,7 +4339,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>259</v>
       </c>
@@ -4339,7 +4347,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>260</v>
       </c>
@@ -4347,7 +4355,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>261</v>
       </c>
@@ -4355,7 +4363,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>262</v>
       </c>
@@ -4363,7 +4371,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>263</v>
       </c>
@@ -4371,23 +4379,23 @@
         <v>404</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>264</v>
       </c>
       <c r="O29" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>2</v>
       </c>
       <c r="O30" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -4395,7 +4403,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>265</v>
       </c>
@@ -4403,7 +4411,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>266</v>
       </c>
@@ -4411,7 +4419,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>267</v>
       </c>
@@ -4419,7 +4427,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>268</v>
       </c>
@@ -4427,7 +4435,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>269</v>
       </c>
@@ -4435,7 +4443,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>270</v>
       </c>
@@ -4443,7 +4451,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>271</v>
       </c>
@@ -4451,7 +4459,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -4459,7 +4467,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>272</v>
       </c>
@@ -4467,7 +4475,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>273</v>
       </c>
@@ -4475,7 +4483,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>274</v>
       </c>
@@ -4483,7 +4491,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>275</v>
       </c>
@@ -4491,7 +4499,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>276</v>
       </c>
@@ -4499,7 +4507,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>277</v>
       </c>
@@ -4507,7 +4515,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>278</v>
       </c>
@@ -4515,7 +4523,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>279</v>
       </c>
@@ -4523,7 +4531,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>280</v>
       </c>
@@ -4531,7 +4539,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>281</v>
       </c>
@@ -4539,7 +4547,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>282</v>
       </c>
@@ -4547,7 +4555,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>283</v>
       </c>
@@ -4555,7 +4563,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>284</v>
       </c>
@@ -4563,7 +4571,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>285</v>
       </c>
@@ -4571,7 +4579,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>286</v>
       </c>
@@ -4579,7 +4587,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>287</v>
       </c>
@@ -4587,7 +4595,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>288</v>
       </c>
@@ -4595,15 +4603,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>2</v>
       </c>
       <c r="O57" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>289</v>
       </c>
@@ -4611,7 +4619,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>290</v>
       </c>
@@ -4619,7 +4627,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>291</v>
       </c>
@@ -4627,7 +4635,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>292</v>
       </c>
@@ -4635,15 +4643,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>9</v>
       </c>
       <c r="O62" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>293</v>
       </c>
@@ -4651,7 +4659,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>294</v>
       </c>
@@ -4659,15 +4667,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>9</v>
       </c>
       <c r="O65" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>295</v>
       </c>
@@ -4675,7 +4683,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>296</v>
       </c>
@@ -4683,7 +4691,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>297</v>
       </c>
@@ -4691,7 +4699,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>298</v>
       </c>
@@ -4699,7 +4707,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>299</v>
       </c>
@@ -4707,7 +4715,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>300</v>
       </c>
@@ -4715,7 +4723,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>301</v>
       </c>
@@ -4723,7 +4731,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>302</v>
       </c>
@@ -4731,15 +4739,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>59</v>
       </c>
       <c r="O74" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>303</v>
       </c>
@@ -4747,7 +4755,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>304</v>
       </c>
@@ -4755,7 +4763,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>305</v>
       </c>
@@ -4763,7 +4771,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>306</v>
       </c>
@@ -4771,7 +4779,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>307</v>
       </c>
@@ -4779,7 +4787,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>308</v>
       </c>
@@ -4787,7 +4795,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>309</v>
       </c>
@@ -4795,7 +4803,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>310</v>
       </c>
@@ -4803,7 +4811,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>311</v>
       </c>
@@ -4811,7 +4819,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>312</v>
       </c>
@@ -4819,7 +4827,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>313</v>
       </c>
@@ -4827,7 +4835,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>314</v>
       </c>
@@ -4835,7 +4843,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>315</v>
       </c>
@@ -4843,15 +4851,15 @@
         <v>404</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>3</v>
       </c>
       <c r="O88" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>316</v>
       </c>
@@ -4859,7 +4867,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>317</v>
       </c>
@@ -4867,7 +4875,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>318</v>
       </c>
@@ -4875,7 +4883,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>319</v>
       </c>
@@ -4883,7 +4891,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>320</v>
       </c>
@@ -4891,15 +4899,15 @@
         <v>404</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>9</v>
       </c>
       <c r="O94" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>321</v>
       </c>
@@ -4907,7 +4915,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>322</v>
       </c>
@@ -4915,23 +4923,23 @@
         <v>404</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>9</v>
       </c>
       <c r="O97" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>26</v>
       </c>
       <c r="O98" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>323</v>
       </c>
@@ -4939,7 +4947,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>324</v>
       </c>
@@ -4947,15 +4955,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>249</v>
       </c>
       <c r="O101" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>325</v>
       </c>
@@ -4963,7 +4971,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>326</v>
       </c>
@@ -4971,7 +4979,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>327</v>
       </c>
@@ -4979,7 +4987,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>328</v>
       </c>
@@ -4987,7 +4995,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>329</v>
       </c>
@@ -4995,7 +5003,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>330</v>
       </c>
@@ -5003,7 +5011,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>331</v>
       </c>
@@ -5011,7 +5019,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>332</v>
       </c>
@@ -5019,15 +5027,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>14</v>
       </c>
       <c r="O110" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>333</v>
       </c>
@@ -5035,15 +5043,15 @@
         <v>404</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>117</v>
       </c>
       <c r="O112" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>334</v>
       </c>
@@ -5051,7 +5059,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>335</v>
       </c>
@@ -5059,7 +5067,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>336</v>
       </c>
@@ -5067,15 +5075,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>2</v>
       </c>
       <c r="O116" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>337</v>
       </c>
@@ -5083,7 +5091,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>338</v>
       </c>
@@ -5091,7 +5099,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>339</v>
       </c>
@@ -5099,7 +5107,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>340</v>
       </c>
@@ -5107,15 +5115,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>341</v>
       </c>
       <c r="O121" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>342</v>
       </c>
@@ -5123,7 +5131,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>343</v>
       </c>
@@ -5131,7 +5139,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>344</v>
       </c>
@@ -5139,7 +5147,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>345</v>
       </c>
@@ -5147,15 +5155,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>9</v>
       </c>
       <c r="O126" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>346</v>
       </c>
@@ -5163,7 +5171,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>347</v>
       </c>
@@ -5171,7 +5179,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>348</v>
       </c>
@@ -5179,7 +5187,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>349</v>
       </c>
@@ -5187,7 +5195,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>350</v>
       </c>
@@ -5195,7 +5203,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>351</v>
       </c>
@@ -5203,7 +5211,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>352</v>
       </c>
@@ -5211,7 +5219,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>353</v>
       </c>
@@ -5219,15 +5227,15 @@
         <v>404</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>9</v>
       </c>
       <c r="O135" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>354</v>
       </c>
@@ -5235,15 +5243,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>2</v>
       </c>
       <c r="O137" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>355</v>
       </c>
@@ -5251,7 +5259,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>356</v>
       </c>
@@ -5259,7 +5267,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>357</v>
       </c>
@@ -5267,23 +5275,23 @@
         <v>402</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>9</v>
       </c>
       <c r="O141" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>9</v>
       </c>
       <c r="O142" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>358</v>
       </c>
@@ -5291,7 +5299,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>359</v>
       </c>
@@ -5299,15 +5307,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>2</v>
       </c>
       <c r="O145" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>360</v>
       </c>
@@ -5315,7 +5323,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>361</v>
       </c>
@@ -5323,7 +5331,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>362</v>
       </c>
@@ -5331,7 +5339,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>363</v>
       </c>
@@ -5339,7 +5347,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>364</v>
       </c>
@@ -5347,7 +5355,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>365</v>
       </c>
@@ -5355,7 +5363,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>366</v>
       </c>
@@ -5363,7 +5371,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>367</v>
       </c>
@@ -5371,7 +5379,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>368</v>
       </c>
@@ -5379,7 +5387,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>26</v>
       </c>
@@ -5387,7 +5395,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>369</v>
       </c>
@@ -5395,7 +5403,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>370</v>
       </c>
@@ -5403,15 +5411,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>371</v>
       </c>
       <c r="O158" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>372</v>
       </c>
@@ -5419,7 +5427,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>373</v>
       </c>
@@ -5427,15 +5435,15 @@
         <v>404</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>9</v>
       </c>
       <c r="O161" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>374</v>
       </c>
@@ -5443,7 +5451,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>375</v>
       </c>
@@ -5451,7 +5459,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>376</v>
       </c>
@@ -5459,7 +5467,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>377</v>
       </c>
@@ -5467,7 +5475,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>378</v>
       </c>
@@ -5475,15 +5483,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>2</v>
       </c>
       <c r="O167" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>379</v>
       </c>
@@ -5491,7 +5499,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>380</v>
       </c>
@@ -5499,7 +5507,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>381</v>
       </c>
@@ -5507,7 +5515,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>382</v>
       </c>
@@ -5515,7 +5523,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>383</v>
       </c>
@@ -5523,7 +5531,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>384</v>
       </c>
@@ -5531,7 +5539,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>385</v>
       </c>
@@ -5539,7 +5547,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>24</v>
       </c>
@@ -5547,7 +5555,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>386</v>
       </c>
@@ -5555,7 +5563,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>209</v>
       </c>
@@ -5563,7 +5571,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>387</v>
       </c>
@@ -5571,7 +5579,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>388</v>
       </c>
@@ -5579,7 +5587,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>389</v>
       </c>
@@ -5587,15 +5595,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>26</v>
       </c>
       <c r="O181" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>390</v>
       </c>
@@ -5603,7 +5611,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>391</v>
       </c>
@@ -5611,7 +5619,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>392</v>
       </c>
@@ -5619,7 +5627,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>393</v>
       </c>
@@ -5627,7 +5635,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>394</v>
       </c>
@@ -5635,7 +5643,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>395</v>
       </c>
@@ -5643,7 +5651,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>26</v>
       </c>
@@ -5651,7 +5659,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>24</v>
       </c>
@@ -5659,7 +5667,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>396</v>
       </c>
@@ -5667,15 +5675,15 @@
         <v>402</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>9</v>
       </c>
       <c r="O191" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>9</v>
       </c>
@@ -5683,7 +5691,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>24</v>
       </c>
@@ -5691,7 +5699,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>14</v>
       </c>
@@ -5699,7 +5707,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>397</v>
       </c>
@@ -5707,7 +5715,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>398</v>
       </c>
@@ -5715,7 +5723,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>399</v>
       </c>
@@ -5723,7 +5731,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>400</v>
       </c>
@@ -5731,7 +5739,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>343</v>
       </c>
@@ -5739,7 +5747,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>401</v>
       </c>
@@ -5747,12 +5755,12 @@
         <v>402</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>9</v>
       </c>
       <c r="O201" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>

</xml_diff>